<commit_message>
Modifiche login lato server
asd
</commit_message>
<xml_diff>
--- a/documentation/Attivita.xlsx
+++ b/documentation/Attivita.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Data inizio</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Creazione progetto</t>
-  </si>
-  <si>
-    <t>Creazione Login</t>
   </si>
   <si>
     <t xml:space="preserve">Gestione Routing </t>
@@ -96,6 +93,21 @@
       <t>ho creato la cartella server e client. Il progetto ha solo una chiamata axios al server hapi. Ricordarsi di usare sass.</t>
     </r>
   </si>
+  <si>
+    <t>Create le chiamate principali per l'autenticazione fake.</t>
+  </si>
+  <si>
+    <t>Bisogna trovare un modulo per fare un'autenticazione sicura. Bisogna agganciare un DB. Bisogna creare anche un sistema di registrazione al sito</t>
+  </si>
+  <si>
+    <t>Creazione Login FAKE</t>
+  </si>
+  <si>
+    <t>Se l'utente esiste bisogna redirezionare alla home page</t>
+  </si>
+  <si>
+    <t>Routing - passaggio valore a componenti figli</t>
+  </si>
 </sst>
 </file>
 
@@ -128,7 +140,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,12 +153,106 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -158,21 +264,51 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -473,7 +609,7 @@
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -487,73 +623,127 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="75">
-      <c r="B3" s="2">
+      <c r="B3" s="9">
         <v>42724</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="10">
         <v>42725</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5" t="s">
+    </row>
+    <row r="4" spans="2:6" ht="60">
+      <c r="B4" s="13">
+        <v>42726</v>
+      </c>
+      <c r="C4" s="13">
+        <v>42727</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="30">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
passaggi di propaganda e funzioni tra componenti
SimpleList - SimpleRow
</commit_message>
<xml_diff>
--- a/documentation/Attivita.xlsx
+++ b/documentation/Attivita.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Data inizio</t>
   </si>
@@ -108,12 +113,18 @@
   <si>
     <t>Routing - passaggio valore a componenti figli</t>
   </si>
+  <si>
+    <t>Passaggio di proprietà fra componenti</t>
+  </si>
+  <si>
+    <t>In SimpleList / SimpleRow ci sono i passaggi di props e funzioni con l'emissione di eventi al componente padre</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +149,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -173,20 +192,20 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -194,17 +213,17 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -212,10 +231,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -224,47 +243,52 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -311,10 +335,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -605,21 +633,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="17" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="47.1640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
@@ -639,7 +667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="75">
+    <row r="3" spans="2:6" ht="56">
       <c r="B3" s="9">
         <v>42724</v>
       </c>
@@ -656,7 +684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="60">
+    <row r="4" spans="2:6" ht="42">
       <c r="B4" s="13">
         <v>42726</v>
       </c>
@@ -673,33 +701,39 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="30">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+    <row r="5" spans="2:6" ht="28">
+      <c r="B5" s="9">
+        <v>42730</v>
+      </c>
+      <c r="C5" s="9">
+        <v>42730</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -708,7 +742,7 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -717,17 +751,19 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="2"/>
@@ -737,43 +773,65 @@
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://github.com/Belar/hapi-vue"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
passaggio variabili a componenti
passaggio di variabili e chiamate ad emit
</commit_message>
<xml_diff>
--- a/documentation/Attivita.xlsx
+++ b/documentation/Attivita.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Data inizio</t>
   </si>
@@ -111,13 +111,16 @@
     <t>Se l'utente esiste bisogna redirezionare alla home page</t>
   </si>
   <si>
-    <t>Routing - passaggio valore a componenti figli</t>
-  </si>
-  <si>
     <t>Passaggio di proprietà fra componenti</t>
   </si>
   <si>
     <t>In SimpleList / SimpleRow ci sono i passaggi di props e funzioni con l'emissione di eventi al componente padre</t>
+  </si>
+  <si>
+    <t>Creazione JSON utente</t>
+  </si>
+  <si>
+    <t>Routing - passaggio valore a componenti figli - da pulire</t>
   </si>
 </sst>
 </file>
@@ -159,7 +162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +181,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -288,7 +297,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -336,6 +345,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -634,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F13"/>
+  <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -709,40 +727,42 @@
         <v>42730</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="17">
+        <v>42732</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -751,7 +771,7 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -760,17 +780,19 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="2"/>
@@ -780,13 +802,20 @@
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
documentazione aggiornata ma da modificare
asp
</commit_message>
<xml_diff>
--- a/documentation/Attivita.xlsx
+++ b/documentation/Attivita.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Data inizio</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Routing - passaggio valore a componenti figli - non mi è ancora chiarissimo come funziona il routing ma l'ho fatto funzionare</t>
+  </si>
+  <si>
+    <t>gestione v-if sui template e aggiornamento vue</t>
+  </si>
+  <si>
+    <t>Aggiornate tutte le librerie di vue. V-if sui template funziona solo all'interno di un template container</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +187,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -283,7 +295,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -291,8 +303,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -306,9 +319,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -345,10 +355,26 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -642,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -659,33 +685,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="56">
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>42724</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>42725</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -693,105 +719,115 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="42">
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>42726</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="12">
         <v>42727</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="28">
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>42730</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>42730</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="2:6" ht="42">
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>42732</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <v>42734</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+    <row r="7" spans="2:6" ht="28">
+      <c r="B7" s="17">
+        <v>42734</v>
+      </c>
+      <c r="C7" s="17">
+        <v>42736</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="19">
+        <v>42736</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="21"/>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="2"/>
@@ -801,13 +837,20 @@
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Documentazione + data nei post
aggiunti e sistemati alcuni json
sistemato il post ed aggiunta la data
incluso momentjs libreria per le date
aggiornato l'xls con le cose da fare/fatte
</commit_message>
<xml_diff>
--- a/documentation/Attivita.xlsx
+++ b/documentation/Attivita.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Data inizio</t>
   </si>
@@ -129,7 +129,55 @@
     <t>Aggiornate tutte le librerie di vue. V-if sui template funziona solo all'interno di un template container</t>
   </si>
   <si>
-    <t>Creazione Post</t>
+    <t>Creazione Post: data</t>
+  </si>
+  <si>
+    <t>Creazione Post: utente</t>
+  </si>
+  <si>
+    <t>Creazione Post: livello onda</t>
+  </si>
+  <si>
+    <t>Creazione Post: foto</t>
+  </si>
+  <si>
+    <t>Creazione Post: breve didascalia</t>
+  </si>
+  <si>
+    <t>l'username dell'utente deve essere linkabile</t>
+  </si>
+  <si>
+    <t>Creazione Post: segnala post</t>
+  </si>
+  <si>
+    <t>si può segnalare un post se la foto è sbagliata</t>
+  </si>
+  <si>
+    <t>segna lo stato dell'onda piatto/appena mosso/ mosso / moltomosso ed il tooltip deve mostrare la leggenda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il messaggio deve essere brevissimo, max 50? 70? Deve mostrare i caratteri rimanenti </t>
+  </si>
+  <si>
+    <t>la foto deve avere un immagine di dimensione fissa</t>
+  </si>
+  <si>
+    <t>copiare meteo.it</t>
+  </si>
+  <si>
+    <t>cerchia utente come quella che fa Sacha, tipo gruppo privato di FB</t>
+  </si>
+  <si>
+    <t>Creazione Post: gestire la visibilità del post</t>
+  </si>
+  <si>
+    <t>formato esteso della data nella lingua</t>
+  </si>
+  <si>
+    <t>bisognerà capire cosa si può vedere dell'utente</t>
+  </si>
+  <si>
+    <t>copiare ove possibile FB - Ho utilizzato moment.js libreria di node</t>
   </si>
 </sst>
 </file>
@@ -197,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -215,80 +263,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -308,73 +284,61 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -674,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F15"/>
+  <dimension ref="B2:F208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -691,47 +655,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="75">
-      <c r="B3" s="8">
+      <c r="B3" s="13">
         <v>42724</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="13">
         <v>42725</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="60">
-      <c r="B4" s="12">
+      <c r="B4" s="13">
         <v>42726</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="13">
         <v>42727</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="14" t="s">
@@ -742,129 +706,1524 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="45">
-      <c r="B5" s="8">
+      <c r="B5" s="13">
         <v>42730</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="13">
         <v>42730</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="2:6" ht="45">
-      <c r="B6" s="12">
+      <c r="B6" s="13">
         <v>42732</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="13">
         <v>42734</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="45">
-      <c r="B7" s="17">
+      <c r="B7" s="13">
         <v>42734</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="13">
         <v>42736</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="17">
+      <c r="B8" s="2">
         <v>42736</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="2">
         <v>42738</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="20"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="19">
+      <c r="B12" s="16">
         <v>42738</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="19">
-        <v>42738</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="2:6" ht="30">
+      <c r="B13" s="13">
+        <v>42740</v>
+      </c>
+      <c r="C13" s="13">
+        <v>42740</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="E13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
+      <c r="B14" s="16">
+        <v>42740</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="45">
+      <c r="B15" s="16">
+        <v>42740</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="30">
+      <c r="B16" s="16">
+        <v>42740</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" ht="30">
+      <c r="B17" s="16">
+        <v>42740</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="16">
+        <v>42740</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="2:6" ht="30">
+      <c r="B19" s="5"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="16"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="2:6" ht="45">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="2:6">
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+    </row>
+    <row r="61" spans="2:6">
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+    </row>
+    <row r="62" spans="2:6">
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+    </row>
+    <row r="76" spans="2:6">
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+    </row>
+    <row r="77" spans="2:6">
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+    </row>
+    <row r="79" spans="2:6">
+      <c r="B79" s="11"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+    </row>
+    <row r="80" spans="2:6">
+      <c r="B80" s="11"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+    </row>
+    <row r="81" spans="2:6">
+      <c r="B81" s="11"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+    </row>
+    <row r="82" spans="2:6">
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+    </row>
+    <row r="83" spans="2:6">
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+    </row>
+    <row r="84" spans="2:6">
+      <c r="B84" s="11"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+    </row>
+    <row r="85" spans="2:6">
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+    </row>
+    <row r="86" spans="2:6">
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+    </row>
+    <row r="87" spans="2:6">
+      <c r="B87" s="11"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+    </row>
+    <row r="88" spans="2:6">
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11"/>
+    </row>
+    <row r="89" spans="2:6">
+      <c r="B89" s="11"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
+    </row>
+    <row r="90" spans="2:6">
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+    </row>
+    <row r="91" spans="2:6">
+      <c r="B91" s="11"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+    </row>
+    <row r="92" spans="2:6">
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+    </row>
+    <row r="93" spans="2:6">
+      <c r="B93" s="11"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
+    </row>
+    <row r="94" spans="2:6">
+      <c r="B94" s="11"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+    </row>
+    <row r="95" spans="2:6">
+      <c r="B95" s="11"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="11"/>
+    </row>
+    <row r="96" spans="2:6">
+      <c r="B96" s="11"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="11"/>
+      <c r="E96" s="11"/>
+      <c r="F96" s="11"/>
+    </row>
+    <row r="97" spans="2:6">
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+    </row>
+    <row r="98" spans="2:6">
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11"/>
+    </row>
+    <row r="99" spans="2:6">
+      <c r="B99" s="11"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11"/>
+    </row>
+    <row r="100" spans="2:6">
+      <c r="B100" s="11"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
+      <c r="E100" s="11"/>
+      <c r="F100" s="11"/>
+    </row>
+    <row r="101" spans="2:6">
+      <c r="B101" s="11"/>
+      <c r="C101" s="11"/>
+      <c r="D101" s="11"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="11"/>
+    </row>
+    <row r="102" spans="2:6">
+      <c r="B102" s="11"/>
+      <c r="C102" s="11"/>
+      <c r="D102" s="11"/>
+      <c r="E102" s="11"/>
+      <c r="F102" s="11"/>
+    </row>
+    <row r="103" spans="2:6">
+      <c r="B103" s="11"/>
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
+      <c r="E103" s="11"/>
+      <c r="F103" s="11"/>
+    </row>
+    <row r="104" spans="2:6">
+      <c r="B104" s="11"/>
+      <c r="C104" s="11"/>
+      <c r="D104" s="11"/>
+      <c r="E104" s="11"/>
+      <c r="F104" s="11"/>
+    </row>
+    <row r="105" spans="2:6">
+      <c r="B105" s="11"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11"/>
+      <c r="E105" s="11"/>
+      <c r="F105" s="11"/>
+    </row>
+    <row r="106" spans="2:6">
+      <c r="B106" s="11"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="11"/>
+      <c r="E106" s="11"/>
+      <c r="F106" s="11"/>
+    </row>
+    <row r="107" spans="2:6">
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
+    </row>
+    <row r="108" spans="2:6">
+      <c r="B108" s="11"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
+    </row>
+    <row r="109" spans="2:6">
+      <c r="B109" s="11"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11"/>
+    </row>
+    <row r="110" spans="2:6">
+      <c r="B110" s="11"/>
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="11"/>
+    </row>
+    <row r="111" spans="2:6">
+      <c r="B111" s="11"/>
+      <c r="C111" s="11"/>
+      <c r="D111" s="11"/>
+      <c r="E111" s="11"/>
+      <c r="F111" s="11"/>
+    </row>
+    <row r="112" spans="2:6">
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+      <c r="E112" s="11"/>
+      <c r="F112" s="11"/>
+    </row>
+    <row r="113" spans="2:6">
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
+      <c r="E113" s="11"/>
+      <c r="F113" s="11"/>
+    </row>
+    <row r="114" spans="2:6">
+      <c r="B114" s="11"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="11"/>
+      <c r="F114" s="11"/>
+    </row>
+    <row r="115" spans="2:6">
+      <c r="B115" s="11"/>
+      <c r="C115" s="11"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="11"/>
+      <c r="F115" s="11"/>
+    </row>
+    <row r="116" spans="2:6">
+      <c r="B116" s="11"/>
+      <c r="C116" s="11"/>
+      <c r="D116" s="11"/>
+      <c r="E116" s="11"/>
+      <c r="F116" s="11"/>
+    </row>
+    <row r="117" spans="2:6">
+      <c r="B117" s="11"/>
+      <c r="C117" s="11"/>
+      <c r="D117" s="11"/>
+      <c r="E117" s="11"/>
+      <c r="F117" s="11"/>
+    </row>
+    <row r="118" spans="2:6">
+      <c r="B118" s="11"/>
+      <c r="C118" s="11"/>
+      <c r="D118" s="11"/>
+      <c r="E118" s="11"/>
+      <c r="F118" s="11"/>
+    </row>
+    <row r="119" spans="2:6">
+      <c r="B119" s="11"/>
+      <c r="C119" s="11"/>
+      <c r="D119" s="11"/>
+      <c r="E119" s="11"/>
+      <c r="F119" s="11"/>
+    </row>
+    <row r="120" spans="2:6">
+      <c r="B120" s="11"/>
+      <c r="C120" s="11"/>
+      <c r="D120" s="11"/>
+      <c r="E120" s="11"/>
+      <c r="F120" s="11"/>
+    </row>
+    <row r="121" spans="2:6">
+      <c r="B121" s="11"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
+      <c r="E121" s="11"/>
+      <c r="F121" s="11"/>
+    </row>
+    <row r="122" spans="2:6">
+      <c r="B122" s="11"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="11"/>
+      <c r="E122" s="11"/>
+      <c r="F122" s="11"/>
+    </row>
+    <row r="123" spans="2:6">
+      <c r="B123" s="11"/>
+      <c r="C123" s="11"/>
+      <c r="D123" s="11"/>
+      <c r="E123" s="11"/>
+      <c r="F123" s="11"/>
+    </row>
+    <row r="124" spans="2:6">
+      <c r="B124" s="11"/>
+      <c r="C124" s="11"/>
+      <c r="D124" s="11"/>
+      <c r="E124" s="11"/>
+      <c r="F124" s="11"/>
+    </row>
+    <row r="125" spans="2:6">
+      <c r="B125" s="11"/>
+      <c r="C125" s="11"/>
+      <c r="D125" s="11"/>
+      <c r="E125" s="11"/>
+      <c r="F125" s="11"/>
+    </row>
+    <row r="126" spans="2:6">
+      <c r="B126" s="11"/>
+      <c r="C126" s="11"/>
+      <c r="D126" s="11"/>
+      <c r="E126" s="11"/>
+      <c r="F126" s="11"/>
+    </row>
+    <row r="127" spans="2:6">
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
+      <c r="E127" s="11"/>
+      <c r="F127" s="11"/>
+    </row>
+    <row r="128" spans="2:6">
+      <c r="B128" s="11"/>
+      <c r="C128" s="11"/>
+      <c r="D128" s="11"/>
+      <c r="E128" s="11"/>
+      <c r="F128" s="11"/>
+    </row>
+    <row r="129" spans="2:6">
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
+      <c r="E129" s="11"/>
+      <c r="F129" s="11"/>
+    </row>
+    <row r="130" spans="2:6">
+      <c r="B130" s="11"/>
+      <c r="C130" s="11"/>
+      <c r="D130" s="11"/>
+      <c r="E130" s="11"/>
+      <c r="F130" s="11"/>
+    </row>
+    <row r="131" spans="2:6">
+      <c r="B131" s="11"/>
+      <c r="C131" s="11"/>
+      <c r="D131" s="11"/>
+      <c r="E131" s="11"/>
+      <c r="F131" s="11"/>
+    </row>
+    <row r="132" spans="2:6">
+      <c r="B132" s="11"/>
+      <c r="C132" s="11"/>
+      <c r="D132" s="11"/>
+      <c r="E132" s="11"/>
+      <c r="F132" s="11"/>
+    </row>
+    <row r="133" spans="2:6">
+      <c r="B133" s="11"/>
+      <c r="C133" s="11"/>
+      <c r="D133" s="11"/>
+      <c r="E133" s="11"/>
+      <c r="F133" s="11"/>
+    </row>
+    <row r="134" spans="2:6">
+      <c r="B134" s="11"/>
+      <c r="C134" s="11"/>
+      <c r="D134" s="11"/>
+      <c r="E134" s="11"/>
+      <c r="F134" s="11"/>
+    </row>
+    <row r="135" spans="2:6">
+      <c r="B135" s="11"/>
+      <c r="C135" s="11"/>
+      <c r="D135" s="11"/>
+      <c r="E135" s="11"/>
+      <c r="F135" s="11"/>
+    </row>
+    <row r="136" spans="2:6">
+      <c r="B136" s="11"/>
+      <c r="C136" s="11"/>
+      <c r="D136" s="11"/>
+      <c r="E136" s="11"/>
+      <c r="F136" s="11"/>
+    </row>
+    <row r="137" spans="2:6">
+      <c r="B137" s="11"/>
+      <c r="C137" s="11"/>
+      <c r="D137" s="11"/>
+      <c r="E137" s="11"/>
+      <c r="F137" s="11"/>
+    </row>
+    <row r="138" spans="2:6">
+      <c r="B138" s="11"/>
+      <c r="C138" s="11"/>
+      <c r="D138" s="11"/>
+      <c r="E138" s="11"/>
+      <c r="F138" s="11"/>
+    </row>
+    <row r="139" spans="2:6">
+      <c r="B139" s="11"/>
+      <c r="C139" s="11"/>
+      <c r="D139" s="11"/>
+      <c r="E139" s="11"/>
+      <c r="F139" s="11"/>
+    </row>
+    <row r="140" spans="2:6">
+      <c r="B140" s="11"/>
+      <c r="C140" s="11"/>
+      <c r="D140" s="11"/>
+      <c r="E140" s="11"/>
+      <c r="F140" s="11"/>
+    </row>
+    <row r="141" spans="2:6">
+      <c r="B141" s="11"/>
+      <c r="C141" s="11"/>
+      <c r="D141" s="11"/>
+      <c r="E141" s="11"/>
+      <c r="F141" s="11"/>
+    </row>
+    <row r="142" spans="2:6">
+      <c r="B142" s="11"/>
+      <c r="C142" s="11"/>
+      <c r="D142" s="11"/>
+      <c r="E142" s="11"/>
+      <c r="F142" s="11"/>
+    </row>
+    <row r="143" spans="2:6">
+      <c r="B143" s="11"/>
+      <c r="C143" s="11"/>
+      <c r="D143" s="11"/>
+      <c r="E143" s="11"/>
+      <c r="F143" s="11"/>
+    </row>
+    <row r="144" spans="2:6">
+      <c r="B144" s="11"/>
+      <c r="C144" s="11"/>
+      <c r="D144" s="11"/>
+      <c r="E144" s="11"/>
+      <c r="F144" s="11"/>
+    </row>
+    <row r="145" spans="2:6">
+      <c r="B145" s="11"/>
+      <c r="C145" s="11"/>
+      <c r="D145" s="11"/>
+      <c r="E145" s="11"/>
+      <c r="F145" s="11"/>
+    </row>
+    <row r="146" spans="2:6">
+      <c r="B146" s="11"/>
+      <c r="C146" s="11"/>
+      <c r="D146" s="11"/>
+      <c r="E146" s="11"/>
+      <c r="F146" s="11"/>
+    </row>
+    <row r="147" spans="2:6">
+      <c r="B147" s="11"/>
+      <c r="C147" s="11"/>
+      <c r="D147" s="11"/>
+      <c r="E147" s="11"/>
+      <c r="F147" s="11"/>
+    </row>
+    <row r="148" spans="2:6">
+      <c r="B148" s="11"/>
+      <c r="C148" s="11"/>
+      <c r="D148" s="11"/>
+      <c r="E148" s="11"/>
+      <c r="F148" s="11"/>
+    </row>
+    <row r="149" spans="2:6">
+      <c r="B149" s="11"/>
+      <c r="C149" s="11"/>
+      <c r="D149" s="11"/>
+      <c r="E149" s="11"/>
+      <c r="F149" s="11"/>
+    </row>
+    <row r="150" spans="2:6">
+      <c r="B150" s="11"/>
+      <c r="C150" s="11"/>
+      <c r="D150" s="11"/>
+      <c r="E150" s="11"/>
+      <c r="F150" s="11"/>
+    </row>
+    <row r="151" spans="2:6">
+      <c r="B151" s="11"/>
+      <c r="C151" s="11"/>
+      <c r="D151" s="11"/>
+      <c r="E151" s="11"/>
+      <c r="F151" s="11"/>
+    </row>
+    <row r="152" spans="2:6">
+      <c r="B152" s="11"/>
+      <c r="C152" s="11"/>
+      <c r="D152" s="11"/>
+      <c r="E152" s="11"/>
+      <c r="F152" s="11"/>
+    </row>
+    <row r="153" spans="2:6">
+      <c r="B153" s="11"/>
+      <c r="C153" s="11"/>
+      <c r="D153" s="11"/>
+      <c r="E153" s="11"/>
+      <c r="F153" s="11"/>
+    </row>
+    <row r="154" spans="2:6">
+      <c r="B154" s="11"/>
+      <c r="C154" s="11"/>
+      <c r="D154" s="11"/>
+      <c r="E154" s="11"/>
+      <c r="F154" s="11"/>
+    </row>
+    <row r="155" spans="2:6">
+      <c r="B155" s="11"/>
+      <c r="C155" s="11"/>
+      <c r="D155" s="11"/>
+      <c r="E155" s="11"/>
+      <c r="F155" s="11"/>
+    </row>
+    <row r="156" spans="2:6">
+      <c r="B156" s="11"/>
+      <c r="C156" s="11"/>
+      <c r="D156" s="11"/>
+      <c r="E156" s="11"/>
+      <c r="F156" s="11"/>
+    </row>
+    <row r="157" spans="2:6">
+      <c r="B157" s="11"/>
+      <c r="C157" s="11"/>
+      <c r="D157" s="11"/>
+      <c r="E157" s="11"/>
+      <c r="F157" s="11"/>
+    </row>
+    <row r="158" spans="2:6">
+      <c r="B158" s="11"/>
+      <c r="C158" s="11"/>
+      <c r="D158" s="11"/>
+      <c r="E158" s="11"/>
+      <c r="F158" s="11"/>
+    </row>
+    <row r="159" spans="2:6">
+      <c r="B159" s="11"/>
+      <c r="C159" s="11"/>
+      <c r="D159" s="11"/>
+      <c r="E159" s="11"/>
+      <c r="F159" s="11"/>
+    </row>
+    <row r="160" spans="2:6">
+      <c r="B160" s="11"/>
+      <c r="C160" s="11"/>
+      <c r="D160" s="11"/>
+      <c r="E160" s="11"/>
+      <c r="F160" s="11"/>
+    </row>
+    <row r="161" spans="2:6">
+      <c r="B161" s="11"/>
+      <c r="C161" s="11"/>
+      <c r="D161" s="11"/>
+      <c r="E161" s="11"/>
+      <c r="F161" s="11"/>
+    </row>
+    <row r="162" spans="2:6">
+      <c r="B162" s="11"/>
+      <c r="C162" s="11"/>
+      <c r="D162" s="11"/>
+      <c r="E162" s="11"/>
+      <c r="F162" s="11"/>
+    </row>
+    <row r="163" spans="2:6">
+      <c r="B163" s="11"/>
+      <c r="C163" s="11"/>
+      <c r="D163" s="11"/>
+      <c r="E163" s="11"/>
+      <c r="F163" s="11"/>
+    </row>
+    <row r="164" spans="2:6">
+      <c r="B164" s="11"/>
+      <c r="C164" s="11"/>
+      <c r="D164" s="11"/>
+      <c r="E164" s="11"/>
+      <c r="F164" s="11"/>
+    </row>
+    <row r="165" spans="2:6">
+      <c r="B165" s="11"/>
+      <c r="C165" s="11"/>
+      <c r="D165" s="11"/>
+      <c r="E165" s="11"/>
+      <c r="F165" s="11"/>
+    </row>
+    <row r="166" spans="2:6">
+      <c r="B166" s="11"/>
+      <c r="C166" s="11"/>
+      <c r="D166" s="11"/>
+      <c r="E166" s="11"/>
+      <c r="F166" s="11"/>
+    </row>
+    <row r="167" spans="2:6">
+      <c r="B167" s="11"/>
+      <c r="C167" s="11"/>
+      <c r="D167" s="11"/>
+      <c r="E167" s="11"/>
+      <c r="F167" s="11"/>
+    </row>
+    <row r="168" spans="2:6">
+      <c r="B168" s="11"/>
+      <c r="C168" s="11"/>
+      <c r="D168" s="11"/>
+      <c r="E168" s="11"/>
+      <c r="F168" s="11"/>
+    </row>
+    <row r="169" spans="2:6">
+      <c r="B169" s="11"/>
+      <c r="C169" s="11"/>
+      <c r="D169" s="11"/>
+      <c r="E169" s="11"/>
+      <c r="F169" s="11"/>
+    </row>
+    <row r="170" spans="2:6">
+      <c r="B170" s="11"/>
+      <c r="C170" s="11"/>
+      <c r="D170" s="11"/>
+      <c r="E170" s="11"/>
+      <c r="F170" s="11"/>
+    </row>
+    <row r="171" spans="2:6">
+      <c r="B171" s="11"/>
+      <c r="C171" s="11"/>
+      <c r="D171" s="11"/>
+      <c r="E171" s="11"/>
+      <c r="F171" s="11"/>
+    </row>
+    <row r="172" spans="2:6">
+      <c r="B172" s="11"/>
+      <c r="C172" s="11"/>
+      <c r="D172" s="11"/>
+      <c r="E172" s="11"/>
+      <c r="F172" s="11"/>
+    </row>
+    <row r="173" spans="2:6">
+      <c r="B173" s="11"/>
+      <c r="C173" s="11"/>
+      <c r="D173" s="11"/>
+      <c r="E173" s="11"/>
+      <c r="F173" s="11"/>
+    </row>
+    <row r="174" spans="2:6">
+      <c r="B174" s="11"/>
+      <c r="C174" s="11"/>
+      <c r="D174" s="11"/>
+      <c r="E174" s="11"/>
+      <c r="F174" s="11"/>
+    </row>
+    <row r="175" spans="2:6">
+      <c r="B175" s="11"/>
+      <c r="C175" s="11"/>
+      <c r="D175" s="11"/>
+      <c r="E175" s="11"/>
+      <c r="F175" s="11"/>
+    </row>
+    <row r="176" spans="2:6">
+      <c r="B176" s="11"/>
+      <c r="C176" s="11"/>
+      <c r="D176" s="11"/>
+      <c r="E176" s="11"/>
+      <c r="F176" s="11"/>
+    </row>
+    <row r="177" spans="2:6">
+      <c r="B177" s="11"/>
+      <c r="C177" s="11"/>
+      <c r="D177" s="11"/>
+      <c r="E177" s="11"/>
+      <c r="F177" s="11"/>
+    </row>
+    <row r="178" spans="2:6">
+      <c r="B178" s="11"/>
+      <c r="C178" s="11"/>
+      <c r="D178" s="11"/>
+      <c r="E178" s="11"/>
+      <c r="F178" s="11"/>
+    </row>
+    <row r="179" spans="2:6">
+      <c r="B179" s="11"/>
+      <c r="C179" s="11"/>
+      <c r="D179" s="11"/>
+      <c r="E179" s="11"/>
+      <c r="F179" s="11"/>
+    </row>
+    <row r="180" spans="2:6">
+      <c r="B180" s="11"/>
+      <c r="C180" s="11"/>
+      <c r="D180" s="11"/>
+      <c r="E180" s="11"/>
+      <c r="F180" s="11"/>
+    </row>
+    <row r="181" spans="2:6">
+      <c r="B181" s="11"/>
+      <c r="C181" s="11"/>
+      <c r="D181" s="11"/>
+      <c r="E181" s="11"/>
+      <c r="F181" s="11"/>
+    </row>
+    <row r="182" spans="2:6">
+      <c r="B182" s="11"/>
+      <c r="C182" s="11"/>
+      <c r="D182" s="11"/>
+      <c r="E182" s="11"/>
+      <c r="F182" s="11"/>
+    </row>
+    <row r="183" spans="2:6">
+      <c r="B183" s="11"/>
+      <c r="C183" s="11"/>
+      <c r="D183" s="11"/>
+      <c r="E183" s="11"/>
+      <c r="F183" s="11"/>
+    </row>
+    <row r="184" spans="2:6">
+      <c r="B184" s="11"/>
+      <c r="C184" s="11"/>
+      <c r="D184" s="11"/>
+      <c r="E184" s="11"/>
+      <c r="F184" s="11"/>
+    </row>
+    <row r="185" spans="2:6">
+      <c r="B185" s="11"/>
+      <c r="C185" s="11"/>
+      <c r="D185" s="11"/>
+      <c r="E185" s="11"/>
+      <c r="F185" s="11"/>
+    </row>
+    <row r="186" spans="2:6">
+      <c r="B186" s="11"/>
+      <c r="C186" s="11"/>
+      <c r="D186" s="11"/>
+      <c r="E186" s="11"/>
+      <c r="F186" s="11"/>
+    </row>
+    <row r="187" spans="2:6">
+      <c r="B187" s="11"/>
+      <c r="C187" s="11"/>
+      <c r="D187" s="11"/>
+      <c r="E187" s="11"/>
+      <c r="F187" s="11"/>
+    </row>
+    <row r="188" spans="2:6">
+      <c r="B188" s="11"/>
+      <c r="C188" s="11"/>
+      <c r="D188" s="11"/>
+      <c r="E188" s="11"/>
+      <c r="F188" s="11"/>
+    </row>
+    <row r="189" spans="2:6">
+      <c r="B189" s="11"/>
+      <c r="C189" s="11"/>
+      <c r="D189" s="11"/>
+      <c r="E189" s="11"/>
+      <c r="F189" s="11"/>
+    </row>
+    <row r="190" spans="2:6">
+      <c r="B190" s="11"/>
+      <c r="C190" s="11"/>
+      <c r="D190" s="11"/>
+      <c r="E190" s="11"/>
+      <c r="F190" s="11"/>
+    </row>
+    <row r="191" spans="2:6">
+      <c r="B191" s="11"/>
+      <c r="C191" s="11"/>
+      <c r="D191" s="11"/>
+      <c r="E191" s="11"/>
+      <c r="F191" s="11"/>
+    </row>
+    <row r="192" spans="2:6">
+      <c r="B192" s="11"/>
+      <c r="C192" s="11"/>
+      <c r="D192" s="11"/>
+      <c r="E192" s="11"/>
+      <c r="F192" s="11"/>
+    </row>
+    <row r="193" spans="2:6">
+      <c r="B193" s="11"/>
+      <c r="C193" s="11"/>
+      <c r="D193" s="11"/>
+      <c r="E193" s="11"/>
+      <c r="F193" s="11"/>
+    </row>
+    <row r="194" spans="2:6">
+      <c r="B194" s="11"/>
+      <c r="C194" s="11"/>
+      <c r="D194" s="11"/>
+      <c r="E194" s="11"/>
+      <c r="F194" s="11"/>
+    </row>
+    <row r="195" spans="2:6">
+      <c r="B195" s="11"/>
+      <c r="C195" s="11"/>
+      <c r="D195" s="11"/>
+      <c r="E195" s="11"/>
+      <c r="F195" s="11"/>
+    </row>
+    <row r="196" spans="2:6">
+      <c r="B196" s="11"/>
+      <c r="C196" s="11"/>
+      <c r="D196" s="11"/>
+      <c r="E196" s="11"/>
+      <c r="F196" s="11"/>
+    </row>
+    <row r="197" spans="2:6">
+      <c r="B197" s="11"/>
+      <c r="C197" s="11"/>
+      <c r="D197" s="11"/>
+      <c r="E197" s="11"/>
+      <c r="F197" s="11"/>
+    </row>
+    <row r="198" spans="2:6">
+      <c r="B198" s="11"/>
+      <c r="C198" s="11"/>
+      <c r="D198" s="11"/>
+      <c r="E198" s="11"/>
+      <c r="F198" s="11"/>
+    </row>
+    <row r="199" spans="2:6">
+      <c r="B199" s="11"/>
+      <c r="C199" s="11"/>
+      <c r="D199" s="11"/>
+      <c r="E199" s="11"/>
+      <c r="F199" s="11"/>
+    </row>
+    <row r="200" spans="2:6">
+      <c r="B200" s="11"/>
+      <c r="C200" s="11"/>
+      <c r="D200" s="11"/>
+      <c r="E200" s="11"/>
+      <c r="F200" s="11"/>
+    </row>
+    <row r="201" spans="2:6">
+      <c r="B201" s="11"/>
+      <c r="C201" s="11"/>
+      <c r="D201" s="11"/>
+      <c r="E201" s="11"/>
+      <c r="F201" s="11"/>
+    </row>
+    <row r="202" spans="2:6">
+      <c r="B202" s="11"/>
+      <c r="C202" s="11"/>
+      <c r="D202" s="11"/>
+      <c r="E202" s="11"/>
+      <c r="F202" s="11"/>
+    </row>
+    <row r="203" spans="2:6">
+      <c r="B203" s="11"/>
+      <c r="C203" s="11"/>
+      <c r="D203" s="11"/>
+      <c r="E203" s="11"/>
+      <c r="F203" s="11"/>
+    </row>
+    <row r="204" spans="2:6">
+      <c r="B204" s="11"/>
+      <c r="C204" s="11"/>
+      <c r="D204" s="11"/>
+      <c r="E204" s="11"/>
+      <c r="F204" s="11"/>
+    </row>
+    <row r="205" spans="2:6">
+      <c r="B205" s="11"/>
+      <c r="C205" s="11"/>
+      <c r="D205" s="11"/>
+      <c r="E205" s="11"/>
+      <c r="F205" s="11"/>
+    </row>
+    <row r="206" spans="2:6">
+      <c r="B206" s="11"/>
+      <c r="C206" s="11"/>
+      <c r="D206" s="11"/>
+      <c r="E206" s="11"/>
+      <c r="F206" s="11"/>
+    </row>
+    <row r="207" spans="2:6">
+      <c r="B207" s="11"/>
+      <c r="C207" s="11"/>
+      <c r="D207" s="11"/>
+      <c r="E207" s="11"/>
+      <c r="F207" s="11"/>
+    </row>
+    <row r="208" spans="2:6">
+      <c r="B208" s="11"/>
+      <c r="C208" s="11"/>
+      <c r="D208" s="11"/>
+      <c r="E208" s="11"/>
+      <c r="F208" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>